<commit_message>
Committing changes to x and y cordinates
</commit_message>
<xml_diff>
--- a/data-munging/Data Quality spreadsheet.xlsx
+++ b/data-munging/Data Quality spreadsheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshitsrivastava/Desktop/NYC Crime/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/General/MS/NYU/Sem I/Courses/Big Data Analytics/Project/NYC-Crime/data-munging/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Invalid</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t xml:space="preserve">Longitude coordinate for Global Coordinate System, WGS 1984, decimal degrees (EPSG 4326) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y_COORD_CD </t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +909,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>45</v>
@@ -929,7 +935,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Adding counts for x and y coordinates
</commit_message>
<xml_diff>
--- a/data-munging/Data Quality spreadsheet.xlsx
+++ b/data-munging/Data Quality spreadsheet.xlsx
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +222,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -255,14 +261,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,12 +295,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,17 +581,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="109.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="3"/>
@@ -896,16 +911,20 @@
         <v>5302218</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7">
+        <v>5384167</v>
+      </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7">
+        <v>195869</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -914,9 +933,13 @@
       <c r="B22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7">
+        <v>5384167</v>
+      </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7">
+        <v>195869</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -947,6 +970,9 @@
       <c r="E24" s="7">
         <v>195869</v>
       </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>